<commit_message>
Added More Certain Missing Elements
Good Job Luke -.-
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bao\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bao\Documents\GitHub\CS273FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -120,7 +120,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -237,8 +236,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-E73C-4956-A097-E15920F34CDD}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -257,8 +257,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-E73C-4956-A097-E15920F34CDD}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -348,6 +349,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E73C-4956-A097-E15920F34CDD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -390,8 +396,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-E73C-4956-A097-E15920F34CDD}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -410,8 +417,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-E73C-4956-A097-E15920F34CDD}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -501,6 +509,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E73C-4956-A097-E15920F34CDD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -549,7 +562,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -669,7 +681,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -767,7 +778,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -879,7 +889,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1498,7 +1507,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 1"/>
+        <xdr:cNvPr id="6" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1529,7 +1544,13 @@
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
-        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD2861C5-F2B2-4648-9325-275D5F2E1241}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
         <cdr:cNvSpPr txBox="1"/>
       </cdr:nvSpPr>
       <cdr:spPr>
@@ -1561,7 +1582,13 @@
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{832F27B5-517E-40AD-8D48-112B4F289801}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
         <cdr:cNvSpPr txBox="1"/>
       </cdr:nvSpPr>
       <cdr:spPr>
@@ -1593,7 +1620,13 @@
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
-        <cdr:cNvPr id="4" name="TextBox 3"/>
+        <cdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84155F36-7047-4D91-BECC-6995ED77B052}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
         <cdr:cNvSpPr txBox="1"/>
       </cdr:nvSpPr>
       <cdr:spPr>
@@ -1625,7 +1658,13 @@
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
-        <cdr:cNvPr id="5" name="TextBox 4"/>
+        <cdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DC3BB96-E6D1-446D-9940-95BE754533C3}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
         <cdr:cNvSpPr txBox="1"/>
       </cdr:nvSpPr>
       <cdr:spPr>
@@ -1725,6 +1764,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1760,6 +1816,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1915,7 +1988,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="A1:I5"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1996,7 +2069,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>14.8104</v>
+        <v>10.2342</v>
       </c>
       <c r="E3">
         <v>10.570600000000001</v>
@@ -2012,7 +2085,7 @@
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I5" si="0">AVERAGE(D3:H3)</f>
-        <v>11.43178</v>
+        <v>10.516540000000001</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>